<commit_message>
Further behavioral analysis, including PD formant analysis
</commit_message>
<xml_diff>
--- a/formant_analysis/ET_formant_freqs.xlsx
+++ b/formant_analysis/ET_formant_freqs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34220" yWindow="760" windowWidth="28800" windowHeight="19080" tabRatio="500"/>
+    <workbookView xWindow="-29280" yWindow="960" windowWidth="28800" windowHeight="19080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -739,7 +739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A405" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I432" sqref="I432:I451"/>
     </sheetView>
   </sheetViews>

</xml_diff>